<commit_message>
Refine five-game design and update documentation
Removed references to a sixth game and virtual events in R scripts and config files to standardize analyses on a five-game design. Updated the pre-analysis plan to clarify tier stratification and randomization procedures, including the use of three-bin grouping when needed. Revised event and study documentation, and deleted obsolete files from the Pre game directory.
</commit_message>
<xml_diff>
--- a/Events/ottawa.xlsx
+++ b/Events/ottawa.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jposada/Library/CloudStorage/Dropbox/I4R/AI vertical/Events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338A32D8-B63D-FA40-8D68-2C4A4B5374B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A251BA-E207-8F4A-AE74-06A1546C3FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="28180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="28180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="University of Ottawa Replicatio" sheetId="1" r:id="rId1"/>
     <sheet name="Assignments_20241009_103554" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'University of Ottawa Replicatio'!$A$1:$AJ$94</definedName>
@@ -2076,7 +2077,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2087,6 +2088,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2102,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2111,6 +2118,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2356,9 +2366,9 @@
   </sheetPr>
   <dimension ref="A1:AJ94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4563,113 +4573,113 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
+    <row r="21" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6">
         <v>110019988168</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="7">
         <v>45922.217245370368</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="7">
         <v>45922.218715277777</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="6">
         <v>127</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J21" s="2">
+      <c r="G21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="6">
         <v>270474947</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M21" s="2" t="s">
+      <c r="L21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="N21" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O21" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="P21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q21" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="R21" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="S21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="T21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="U21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="V21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="W21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X21" s="6">
         <v>15</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Y21" s="6">
         <v>66</v>
       </c>
-      <c r="Z21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI21" s="2" t="s">
+      <c r="Z21" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AJ21" s="2" t="s">
+      <c r="AJ21" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10283,113 +10293,113 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="A73" s="2">
+    <row r="73" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="6">
         <v>110020032249</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="7">
         <v>45926.915625000001</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="7">
         <v>45926.917210648149</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="6">
         <v>136</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G73" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J73" s="2">
+      <c r="G73" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J73" s="6">
         <v>270474947</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="K73" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L73" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M73" s="2" t="s">
+      <c r="L73" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M73" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N73" s="2" t="s">
+      <c r="N73" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="O73" s="2" t="s">
+      <c r="O73" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="P73" s="2" t="s">
+      <c r="P73" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q73" s="2" t="s">
+      <c r="Q73" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="R73" s="2" t="s">
+      <c r="R73" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="S73" s="2" t="s">
+      <c r="S73" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="T73" s="2" t="s">
+      <c r="T73" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="U73" s="2" t="s">
+      <c r="U73" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V73" s="2" t="s">
+      <c r="V73" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="W73" s="2" t="s">
+      <c r="W73" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="X73" s="2">
+      <c r="X73" s="6">
         <v>3</v>
       </c>
-      <c r="Y73" s="2">
+      <c r="Y73" s="6">
         <v>100</v>
       </c>
-      <c r="Z73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH73" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI73" s="2" t="s">
+      <c r="Z73" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD73" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG73" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH73" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI73" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="AJ73" s="2" t="s">
+      <c r="AJ73" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -12714,7 +12724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -17195,4 +17205,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4DCD68-A613-4A4C-B27A-EB5AE3F5F874}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor analyses to three expertise tiers and streamline tables
Revised R analysis scripts and pre-analysis plan to use three expertise tiers (Undergraduate, Graduate, Professor/Researcher) instead of five, removed prompt usage as a main outcome, and updated regression specifications and output tables accordingly. Added new metrics for planned and implemented robustness checks, simplified referee outcomes, and removed prompt count simulation and related figures. Updated config and documentation to match new design.
</commit_message>
<xml_diff>
--- a/Events/ottawa.xlsx
+++ b/Events/ottawa.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jposada/Library/CloudStorage/Dropbox/I4R/AI vertical/Events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE59C0EB-3701-C749-A793-1D3AFE78DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B5EF50-6F43-1847-B24B-3A89774BFA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="28180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="51200" windowHeight="28180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="University of Ottawa Replicatio" sheetId="1" r:id="rId1"/>
     <sheet name="Assignments_20241009_152508" sheetId="4" r:id="rId2"/>
+    <sheet name="Dropouts" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'University of Ottawa Replicatio'!$A$1:$AJ$96</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="691">
   <si>
     <t>Response ID</t>
   </si>
@@ -2407,8 +2408,8 @@
   <dimension ref="A1:AJ96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12984,8 +12985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17998,4 +17999,29 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0303CD-B44D-8E46-85D3-C36C3112A483}">
+  <dimension ref="A2:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>